<commit_message>
laatste versie voor kopieren cohorten
</commit_message>
<xml_diff>
--- a/public/cohort/fileExcel/_sjabloon_v3.xlsx
+++ b/public/cohort/fileExcel/_sjabloon_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgnl-my.sharepoint.com/personal/vnr_csg_nl/Documents/SCHOOLdocumenten/CORONA/PTO PTA/cohortproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="338" documentId="11_AD4D7A0C205A6B9A452FA84F5F1974425ADEDD8A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{377BEB92-0722-4072-BDA4-896AE2F7BF8A}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="11_AD4D7A0C205A6B9A452FA84F5F1974425ADEDD8A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{70F05101-AF85-427F-95B5-2E45DBDF5084}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -513,6 +522,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -522,9 +534,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1405,7 +1414,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1431,7 +1440,7 @@
       <c r="C1" s="15"/>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
-      <c r="G1" s="37"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -1440,16 +1449,16 @@
       <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="36" t="str">
+      <c r="G2" s="37" t="str">
         <f ca="1">IF(B14&gt;6,"verouderd PTA",CONCATENATE("Dit is het programma van de huidige ",B6,B14," (cohort ",B7," - ",B9,")"))</f>
         <v>verouderd PTA</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -1629,7 +1638,7 @@
       </c>
       <c r="B10" s="6">
         <f ca="1">NOW()</f>
-        <v>44340.863057407405</v>
+        <v>44341.381435532407</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1702,16 +1711,16 @@
         <v>21</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="G13" s="34" t="str">
+      <c r="G13" s="35" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G4)</f>
         <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 4 (schooljaar  - 1)</v>
       </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
     </row>
     <row r="14" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -1721,13 +1730,13 @@
         <f ca="1">B15+B11-B7</f>
         <v>2024</v>
       </c>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -1923,25 +1932,25 @@
         <v>21</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="G25" s="34" t="str">
+      <c r="G25" s="35" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G16)</f>
         <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 5 (schooljaar 1 - 2)</v>
       </c>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
     </row>
     <row r="26" spans="3:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
     </row>
     <row r="28" spans="3:16" ht="30.75" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="9" t="s">
@@ -2128,28 +2137,28 @@
         <v>21</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="G37" s="34" t="str">
+      <c r="G37" s="35" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G28)</f>
         <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 6 (schooljaar 2 - 1)</v>
       </c>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
     </row>
     <row r="38" spans="3:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="35"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="36"/>
+      <c r="M38" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="SrX3S+ZNQoctHKAEl4ooEqJ3r4tBtF75kCSPVMl9RCxk7BUvQA71JlF2cy7orB5a5+HvCXP+BUo+YzbIklQFYA==" saltValue="+Q/96ROk+k5baqU9EJnmoQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="G37:M37"/>
     <mergeCell ref="G38:M38"/>

</xml_diff>

<commit_message>
Excel - voor cohortkopie
</commit_message>
<xml_diff>
--- a/public/cohort/fileExcel/_sjabloon_v3.xlsx
+++ b/public/cohort/fileExcel/_sjabloon_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgnl-my.sharepoint.com/personal/vnr_csg_nl/Documents/SCHOOLdocumenten/CORONA/PTO PTA/cohortproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="341" documentId="11_AD4D7A0C205A6B9A452FA84F5F1974425ADEDD8A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{70F05101-AF85-427F-95B5-2E45DBDF5084}"/>
+  <xr:revisionPtr revIDLastSave="453" documentId="11_AD4D7A0C205A6B9A452FA84F5F1974425ADEDD8A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0691D06B-C5BB-43EC-8DA5-3E93AC1B3BDB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="65">
   <si>
     <t>statusCode</t>
   </si>
@@ -188,44 +188,550 @@
     <t>hoeft niet gevuld (want geen SE)</t>
   </si>
   <si>
-    <t>niet knippen?</t>
-  </si>
-  <si>
-    <t>geen vormgeving doen</t>
-  </si>
-  <si>
-    <t>tijd in minuten, geen toevoeging</t>
-  </si>
-  <si>
-    <t>laat niet relevante dingen open</t>
-  </si>
-  <si>
-    <t>structuur etc. moet nog weer beveiligd!</t>
-  </si>
-  <si>
     <t>mavo?</t>
   </si>
   <si>
-    <t>niet formatten. Layouten doen wij.</t>
-  </si>
-  <si>
-    <t>zie je iets waarvan je denkt dat het niet klopt! Mail me.</t>
-  </si>
-  <si>
-    <t>niet in oude Excel openen. Op school / in Teams.</t>
-  </si>
-  <si>
-    <t>donkergroen alleen invullen als SE</t>
-  </si>
-  <si>
-    <t>wat betekent naam tabblad: hoe kun je het zien?</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">INSTRUCTIE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>graag uw aandacht voor het volgende:</t>
+    </r>
+  </si>
+  <si>
+    <t>Vorig jaar zijn we overgestapt van de invoer van PTA's via Word naar Excel. Dit was een eerste stap in een groter proces waarbij we toewillen naar het werken met volledige PTA-cohorten: PTA's waarin alle leerjaren van een examengroep staan beschreven. Dit nieuwe invoerdocument is een uitwerking daarvan.</t>
+  </si>
+  <si>
+    <t>COHORTEN en COHORTJAREN</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In dit document zie je tabbladen met namen als </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>A 2019</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>H 2021</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. Dat jaartal slaat op het kalenderjaar waarin een groep start met het schoolexamen (gerekend vanaf mavo-3, havo-4 en VWO-4). Voor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>A 2019</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> gaat het dus om de atheneum-groep die in het schooljaar </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>2019-2020</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in klas 4 zat, in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>2020-2021</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in klas 5 en in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>2021-2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in klas 6. Het volledige </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>cohort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is dan de periode 2019-2022. Het betreft hier dus de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>huidige vwo-5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Als je klikt op een tabblad wordt dit vermeld.</t>
+    </r>
+  </si>
+  <si>
+    <t>SCHRIJFRECHT en leesrecht: CONTROLE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">HEEL BELANGRIJK: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>do's &amp; don'ts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lees dit gedeelte echt even goed door. Vorig jaar hebben we veel nawerk gehad door </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>afwijkende invoer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in het Excelbestand, niet volledig ingevulde gegevens en niet kloppende gegevens. Allereerst: Open dit bestand niet in een verouderde Excel-versie. Open hem op je schoollaptop of een werkstation op school </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>vanuit Teams</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. Download het bestand dus </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>niet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Dit leidt tot ongewenste dubbelingen en inconsistentie. Let daarnaast bij de over op de volgende punten:</t>
+    </r>
+  </si>
+  <si>
+    <t>overzicht aandachtspunten bij het werken met dit document</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Voor de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>huidige vwo-5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> zijn de leerjaren 4 en 5 van het PTA al voorbij en uitgevoerd. Daarom zijn de bijbehorende velden geblokkeerd. Wij hebben alle informatie van het huidige schooljaar overgenomen in dit nieuwe bestand. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Wil je controleren of de gegevens van het huidige schooljaar juist zijn?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Klopt er iets niet? Stuur dan een mailtje naar VNR. Velden voor het komende schooljaar zijn wel beschrijfbaar. Hier vul je het PTA verder in. Net als vorig jaar verwachten we het </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>volledige onderwijsprogramma</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> voor een leerlaag, dus ook de proefwerken en andere opdrachten die niet voor het schoolexamen gelden. Als service hebben we het cohortjaar dat je voor dit schooljaar had ingevuld gekopieerd naar het PTA voor de nieuwe groep.</t>
+    </r>
+  </si>
+  <si>
+    <t>De groene velden zijn beschrijfbaar. De donkergroene velden hoef je alleen in te vullen als er sprake is van een PTA-onderdeel.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wil je iets verplaatsen? Ga alsjeblieft </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>niet knippen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (geen Ctrl-x). Daarmee verwijder je namelijk ook voor jou onzichtbare onderdelen. In plaats daarvan: het meest veilig is even overschrijven, maar als je toch wilt kopiëren: kies dan in het nieuwe veld voor het </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>plakken van waarden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> en delete vervolgens de inhoud van de velden die moeten worden geleegd.</t>
+    </r>
+  </si>
+  <si>
+    <t>Vorig jaar hebben secties soms zelf geprobeerd hun PTA te layouten binnen Excel met b.v. spaties. Doe dit niet. Het PTA wordt uiteindelijk als PDF afgedrukt in een andere layout. Zelf aanpassen heeft dus geen zin, maar zorgt wel voor problemen bij de verdere verwerking!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">De kolommen </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>weging VD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>weging SE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> en </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>duur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> zijn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>numeriek</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. Vul hier alleen getallen in (en dus niet dingen als </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">100 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>, etc.)</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,20 +806,66 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="0" tint="-0.14999847407452621"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="3"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,8 +932,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -439,11 +997,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -521,8 +1094,7 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -534,6 +1106,25 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1202,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BB6D28-398B-4698-A0A3-B23DA82B4117}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,71 +1928,156 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="WOf0LQsboE6wZUxhTrp6vWUPTX/PxW+vApAM6zdPOcGfqvqNuFNYmJEfEBPc31Vp+JEs0x9YELJOz7LGwIuUbA==" saltValue="ss5ASBCr8o3o1bhwu9U1Vw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A11"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="95.140625" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="8"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="161.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="40" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="10" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
-        <v>54</v>
-      </c>
+    <row r="11" spans="1:2" s="37" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="38"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="38"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="38"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="38"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="38"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="38"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="38"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="38"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="38"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="38"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="38"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="38"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="38"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="38"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="38"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="38"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="38"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="mV7BNsQoFesF/gHTqLwFID77XCVLa9wfBt+/qI6NBt8ZJQTq+zXXlgMeU+Yap4FYo3SfLn1U8mRQOMZH2GCMGQ==" saltValue="vl1+j0HvtxTC7FXpJM93Ug==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -1414,7 +2090,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1440,7 +2116,7 @@
       <c r="C1" s="15"/>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
-      <c r="G1" s="34"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -1449,16 +2125,16 @@
       <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="37" t="str">
+      <c r="G2" s="36" t="str">
         <f ca="1">IF(B14&gt;6,"verouderd PTA",CONCATENATE("Dit is het programma van de huidige ",B6,B14," (cohort ",B7," - ",B9,")"))</f>
         <v>verouderd PTA</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -1638,7 +2314,7 @@
       </c>
       <c r="B10" s="6">
         <f ca="1">NOW()</f>
-        <v>44341.381435532407</v>
+        <v>44341.451444791666</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1711,16 +2387,16 @@
         <v>21</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="G13" s="35" t="str">
+      <c r="G13" s="34" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G4)</f>
         <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 4 (schooljaar  - 1)</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
     </row>
     <row r="14" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -1730,17 +2406,17 @@
         <f ca="1">B15+B11-B7</f>
         <v>2024</v>
       </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B15" s="7">
         <f>IF(B6="M",3,4)</f>
@@ -1932,25 +2608,25 @@
         <v>21</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="G25" s="35" t="str">
+      <c r="G25" s="34" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G16)</f>
         <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 5 (schooljaar 1 - 2)</v>
       </c>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
     </row>
     <row r="26" spans="3:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
     </row>
     <row r="28" spans="3:16" ht="30.75" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="9" t="s">
@@ -2137,25 +2813,25 @@
         <v>21</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="G37" s="35" t="str">
+      <c r="G37" s="34" t="str">
         <f>CONCATENATE("Algemene opmerkingen bij het jaarprogramma van  ",G28)</f>
         <v>Algemene opmerkingen bij het jaarprogramma van   leerlaag 6 (schooljaar 2 - 1)</v>
       </c>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="35"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
+      <c r="K37" s="34"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
     </row>
     <row r="38" spans="3:16" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="SrX3S+ZNQoctHKAEl4ooEqJ3r4tBtF75kCSPVMl9RCxk7BUvQA71JlF2cy7orB5a5+HvCXP+BUo+YzbIklQFYA==" saltValue="+Q/96ROk+k5baqU9EJnmoQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>

</xml_diff>